<commit_message>
add frame side B image
</commit_message>
<xml_diff>
--- a/documentation/printed_parts_md_builder.xlsx
+++ b/documentation/printed_parts_md_builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f75adbc1b1328d64/Documents/GitHub/BabyBeltPro/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{C0675C86-CF61-45B1-818F-376B7F2C33E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D2B1B20-C464-4755-9350-D5512DC0306C}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{C0675C86-CF61-45B1-818F-376B7F2C33E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9933B59-C637-430D-8B78-7D9CD434981A}"/>
   <bookViews>
     <workbookView xWindow="1095" yWindow="4455" windowWidth="38700" windowHeight="15345" xr2:uid="{56CCDE47-8BF8-4249-AE9A-3862BA691127}"/>
   </bookViews>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC80A11F-D4A9-4A4B-AA84-1AE963FFD50F}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K36"/>
     </sheetView>
   </sheetViews>
@@ -661,8 +661,8 @@
         <v>[BBProV25fl_scraper](../STLs/Frame/BBProV25fl_scraper.stl)</v>
       </c>
       <c r="E3" t="str">
-        <f>"[!["&amp;LEFT($B3,LEN($B3)-4)&amp;"](./images/printed_parts/"&amp;SUBSTITUTE($C3," ","%20")&amp;"/"&amp;SUBSTITUTE(SUBSTITUTE($B3,".stl",".jpg")," ","%20")&amp;")]"</f>
-        <v>[![BBProV25fl_scraper](./images/printed_parts/Frame/BBProV25fl_scraper.jpg)]</v>
+        <f>"!["&amp;LEFT($B3,LEN($B3)-4)&amp;"](./images/printed_parts/"&amp;SUBSTITUTE($C3," ","%20")&amp;"/"&amp;SUBSTITUTE(SUBSTITUTE($B3,".stl",".jpg")," ","%20")&amp;")"</f>
+        <v>![BBProV25fl_scraper](./images/printed_parts/Frame/BBProV25fl_scraper.jpg)</v>
       </c>
       <c r="F3" t="str">
         <f>$C3</f>
@@ -681,7 +681,7 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_scraper](../STLs/Frame/BBProV25fl_scraper.stl)|[![BBProV25fl_scraper](./images/printed_parts/Frame/BBProV25fl_scraper.jpg)]|Frame|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_scraper](../STLs/Frame/BBProV25fl_scraper.stl)|![BBProV25fl_scraper](./images/printed_parts/Frame/BBProV25fl_scraper.jpg)|Frame|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -701,8 +701,8 @@
         <v>[BBProV25fl_Side-A](../STLs/Frame/BBProV25fl_Side-A.stl)</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E36" si="5">"[!["&amp;LEFT($B4,LEN($B4)-4)&amp;"](./images/printed_parts/"&amp;SUBSTITUTE($C4," ","%20")&amp;"/"&amp;SUBSTITUTE(SUBSTITUTE($B4,".stl",".jpg")," ","%20")&amp;")]"</f>
-        <v>[![BBProV25fl_Side-A](./images/printed_parts/Frame/BBProV25fl_Side-A.jpg)]</v>
+        <f t="shared" ref="E4:E36" si="5">"!["&amp;LEFT($B4,LEN($B4)-4)&amp;"](./images/printed_parts/"&amp;SUBSTITUTE($C4," ","%20")&amp;"/"&amp;SUBSTITUTE(SUBSTITUTE($B4,".stl",".jpg")," ","%20")&amp;")"</f>
+        <v>![BBProV25fl_Side-A](./images/printed_parts/Frame/BBProV25fl_Side-A.jpg)</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F36" si="6">$C4</f>
@@ -721,7 +721,7 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_Side-A](../STLs/Frame/BBProV25fl_Side-A.stl)|[![BBProV25fl_Side-A](./images/printed_parts/Frame/BBProV25fl_Side-A.jpg)]|Frame|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_Side-A](../STLs/Frame/BBProV25fl_Side-A.stl)|![BBProV25fl_Side-A](./images/printed_parts/Frame/BBProV25fl_Side-A.jpg)|Frame|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="5"/>
-        <v>[![BBProV25fl_Side-B](./images/printed_parts/Frame/BBProV25fl_Side-B.jpg)]</v>
+        <v>![BBProV25fl_Side-B](./images/printed_parts/Frame/BBProV25fl_Side-B.jpg)</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="6"/>
@@ -761,7 +761,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_Side-B](../STLs/Frame/BBProV25fl_Side-B.stl)|[![BBProV25fl_Side-B](./images/printed_parts/Frame/BBProV25fl_Side-B.jpg)]|Frame|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_Side-B](../STLs/Frame/BBProV25fl_Side-B.stl)|![BBProV25fl_Side-B](./images/printed_parts/Frame/BBProV25fl_Side-B.jpg)|Frame|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="5"/>
-        <v>[![[s]_BBProV24fl_Screenmount](./images/printed_parts/Frame/[s]_BBProV24fl_Screenmount.jpg)]</v>
+        <v>![[s]_BBProV24fl_Screenmount](./images/printed_parts/Frame/[s]_BBProV24fl_Screenmount.jpg)</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="6"/>
@@ -801,7 +801,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>|[[s]_BBProV24fl_Screenmount](../STLs/Frame/[s]_BBProV24fl_Screenmount.stl)|[![[s]_BBProV24fl_Screenmount](./images/printed_parts/Frame/[s]_BBProV24fl_Screenmount.jpg)]|Frame|Main|Yes|PLA or Better|</v>
+        <v>|[[s]_BBProV24fl_Screenmount](../STLs/Frame/[s]_BBProV24fl_Screenmount.stl)|![[s]_BBProV24fl_Screenmount](./images/printed_parts/Frame/[s]_BBProV24fl_Screenmount.jpg)|Frame|Main|Yes|PLA or Better|</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_YCar_Bam_BeltHolder](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_BeltHolder.jpg)]</v>
+        <v>![[a]_BBProV25fl_YCar_Bam_BeltHolder](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_BeltHolder.jpg)</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="6"/>
@@ -841,7 +841,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_YCar_Bam_BeltHolder](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_BeltHolder.stl)|[![[a]_BBProV25fl_YCar_Bam_BeltHolder](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_BeltHolder.jpg)]|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_YCar_Bam_BeltHolder](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_BeltHolder.stl)|![[a]_BBProV25fl_YCar_Bam_BeltHolder](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_BeltHolder.jpg)|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_YCar_Bam_Fan](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_Fan.jpg)]</v>
+        <v>![[a]_BBProV25fl_YCar_Bam_Fan](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_Fan.jpg)</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="6"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_YCar_Bam_Fan](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_Fan.stl)|[![[a]_BBProV25fl_YCar_Bam_Fan](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_Fan.jpg)]|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_YCar_Bam_Fan](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_Fan.stl)|![[a]_BBProV25fl_YCar_Bam_Fan](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_Fan.jpg)|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_YCar_Bam_SideA](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideA.jpg)]</v>
+        <v>![[a]_BBProV25fl_YCar_Bam_SideA](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideA.jpg)</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="6"/>
@@ -921,7 +921,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_YCar_Bam_SideA](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideA.stl)|[![[a]_BBProV25fl_YCar_Bam_SideA](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideA.jpg)]|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_YCar_Bam_SideA](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideA.stl)|![[a]_BBProV25fl_YCar_Bam_SideA](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideA.jpg)|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_YCar_Bam_SideB](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideB.jpg)]</v>
+        <v>![[a]_BBProV25fl_YCar_Bam_SideB](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideB.jpg)</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="6"/>
@@ -961,7 +961,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_YCar_Bam_SideB](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideB.stl)|[![[a]_BBProV25fl_YCar_Bam_SideB](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideB.jpg)]|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_YCar_Bam_SideB](../STLs/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideB.stl)|![[a]_BBProV25fl_YCar_Bam_SideB](./images/printed_parts/Gantry/Carriage/Bambu/[a]_BBProV25fl_YCar_Bam_SideB.jpg)|Gantry/Carriage/Bambu|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBPro_fanduct](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_fanduct.jpg)]</v>
+        <v>![[a]_BBPro_fanduct](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_fanduct.jpg)</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="6"/>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBPro_fanduct](../STLs/Gantry/Carriage/Revo/[a]_BBPro_fanduct.stl)|[![[a]_BBPro_fanduct](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_fanduct.jpg)]|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBPro_fanduct](../STLs/Gantry/Carriage/Revo/[a]_BBPro_fanduct.stl)|![[a]_BBPro_fanduct](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_fanduct.jpg)|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBPro_partsfanmount](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_partsfanmount.jpg)]</v>
+        <v>![[a]_BBPro_partsfanmount](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_partsfanmount.jpg)</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="6"/>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBPro_partsfanmount](../STLs/Gantry/Carriage/Revo/[a]_BBPro_partsfanmount.stl)|[![[a]_BBPro_partsfanmount](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_partsfanmount.jpg)]|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBPro_partsfanmount](../STLs/Gantry/Carriage/Revo/[a]_BBPro_partsfanmount.stl)|![[a]_BBPro_partsfanmount](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_partsfanmount.jpg)|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBPro_YCar-WireAndBelt_17](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCar-WireAndBelt_17.jpg)]</v>
+        <v>![[a]_BBPro_YCar-WireAndBelt_17](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCar-WireAndBelt_17.jpg)</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="6"/>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBPro_YCar-WireAndBelt_17](../STLs/Gantry/Carriage/Revo/[a]_BBPro_YCar-WireAndBelt_17.stl)|[![[a]_BBPro_YCar-WireAndBelt_17](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCar-WireAndBelt_17.jpg)]|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBPro_YCar-WireAndBelt_17](../STLs/Gantry/Carriage/Revo/[a]_BBPro_YCar-WireAndBelt_17.stl)|![[a]_BBPro_YCar-WireAndBelt_17](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCar-WireAndBelt_17.jpg)|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBPro_YCarLside_A](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_A.jpg)]</v>
+        <v>![[a]_BBPro_YCarLside_A](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_A.jpg)</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="6"/>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBPro_YCarLside_A](../STLs/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_A.stl)|[![[a]_BBPro_YCarLside_A](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_A.jpg)]|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBPro_YCarLside_A](../STLs/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_A.stl)|![[a]_BBPro_YCarLside_A](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_A.jpg)|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBPro_YCarLside_B](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_B.jpg)]</v>
+        <v>![[a]_BBPro_YCarLside_B](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_B.jpg)</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="6"/>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBPro_YCarLside_B](../STLs/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_B.stl)|[![[a]_BBPro_YCarLside_B](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_B.jpg)]|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBPro_YCarLside_B](../STLs/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_B.stl)|![[a]_BBPro_YCarLside_B](./images/printed_parts/Gantry/Carriage/Revo/[a]_BBPro_YCarLside_B.jpg)|Gantry/Carriage/Revo|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="5"/>
-        <v>[![BBProV25fl_X-Carraige](./images/printed_parts/Gantry/X/BBProV25fl_X-Carraige.jpg)]</v>
+        <v>![BBProV25fl_X-Carraige](./images/printed_parts/Gantry/X/BBProV25fl_X-Carraige.jpg)</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="6"/>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_X-Carraige](../STLs/Gantry/X/BBProV25fl_X-Carraige.stl)|[![BBProV25fl_X-Carraige](./images/printed_parts/Gantry/X/BBProV25fl_X-Carraige.jpg)]|Gantry/X|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_X-Carraige](../STLs/Gantry/X/BBProV25fl_X-Carraige.stl)|![BBProV25fl_X-Carraige](./images/printed_parts/Gantry/X/BBProV25fl_X-Carraige.jpg)|Gantry/X|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_pivotArm(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_pivotArm(2x).jpg)]</v>
+        <v>![[a]_BBProV25fl_pivotArm(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_pivotArm(2x).jpg)</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="6"/>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_pivotArm(2x)](../STLs/Gantry/X/[a]_BBProV25fl_pivotArm(2x).stl)|[![[a]_BBProV25fl_pivotArm(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_pivotArm(2x).jpg)]|Gantry/X|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_pivotArm(2x)](../STLs/Gantry/X/[a]_BBProV25fl_pivotArm(2x).stl)|![[a]_BBProV25fl_pivotArm(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_pivotArm(2x).jpg)|Gantry/X|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_XPivotClamp(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XPivotClamp(2x).jpg)]</v>
+        <v>![[a]_BBProV25fl_XPivotClamp(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XPivotClamp(2x).jpg)</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="6"/>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_XPivotClamp(2x)](../STLs/Gantry/X/[a]_BBProV25fl_XPivotClamp(2x).stl)|[![[a]_BBProV25fl_XPivotClamp(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XPivotClamp(2x).jpg)]|Gantry/X|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_XPivotClamp(2x)](../STLs/Gantry/X/[a]_BBProV25fl_XPivotClamp(2x).stl)|![[a]_BBProV25fl_XPivotClamp(2x)](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XPivotClamp(2x).jpg)|Gantry/X|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_XrailMount-SideA](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideA.jpg)]</v>
+        <v>![[a]_BBProV25fl_XrailMount-SideA](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideA.jpg)</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="6"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_XrailMount-SideA](../STLs/Gantry/X/[a]_BBProV25fl_XrailMount-SideA.stl)|[![[a]_BBProV25fl_XrailMount-SideA](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideA.jpg)]|Gantry/X|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_XrailMount-SideA](../STLs/Gantry/X/[a]_BBProV25fl_XrailMount-SideA.stl)|![[a]_BBProV25fl_XrailMount-SideA](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideA.jpg)|Gantry/X|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_XrailMount-SideB](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideB.jpg)]</v>
+        <v>![[a]_BBProV25fl_XrailMount-SideB](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideB.jpg)</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="6"/>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_XrailMount-SideB](../STLs/Gantry/X/[a]_BBProV25fl_XrailMount-SideB.stl)|[![[a]_BBProV25fl_XrailMount-SideB](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideB.jpg)]|Gantry/X|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_XrailMount-SideB](../STLs/Gantry/X/[a]_BBProV25fl_XrailMount-SideB.stl)|![[a]_BBProV25fl_XrailMount-SideB](./images/printed_parts/Gantry/X/[a]_BBProV25fl_XrailMount-SideB.jpg)|Gantry/X|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="5"/>
-        <v>[![BBProV25fl_LinearRailReplacement](./images/printed_parts/Gantry/Y/BBProV25fl_LinearRailReplacement.jpg)]</v>
+        <v>![BBProV25fl_LinearRailReplacement](./images/printed_parts/Gantry/Y/BBProV25fl_LinearRailReplacement.jpg)</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="6"/>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_LinearRailReplacement](../STLs/Gantry/Y/BBProV25fl_LinearRailReplacement.stl)|[![BBProV25fl_LinearRailReplacement](./images/printed_parts/Gantry/Y/BBProV25fl_LinearRailReplacement.jpg)]|Gantry/Y|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_LinearRailReplacement](../STLs/Gantry/Y/BBProV25fl_LinearRailReplacement.stl)|![BBProV25fl_LinearRailReplacement](./images/printed_parts/Gantry/Y/BBProV25fl_LinearRailReplacement.jpg)|Gantry/Y|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="5"/>
-        <v>[![BBProV25fl_RockMonsterNo1YTentionerNut](./images/printed_parts/Gantry/Y/BBProV25fl_RockMonsterNo1YTentionerNut.jpg)]</v>
+        <v>![BBProV25fl_RockMonsterNo1YTentionerNut](./images/printed_parts/Gantry/Y/BBProV25fl_RockMonsterNo1YTentionerNut.jpg)</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="6"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_RockMonsterNo1YTentionerNut](../STLs/Gantry/Y/BBProV25fl_RockMonsterNo1YTentionerNut.stl)|[![BBProV25fl_RockMonsterNo1YTentionerNut](./images/printed_parts/Gantry/Y/BBProV25fl_RockMonsterNo1YTentionerNut.jpg)]|Gantry/Y|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_RockMonsterNo1YTentionerNut](../STLs/Gantry/Y/BBProV25fl_RockMonsterNo1YTentionerNut.stl)|![BBProV25fl_RockMonsterNo1YTentionerNut](./images/printed_parts/Gantry/Y/BBProV25fl_RockMonsterNo1YTentionerNut.jpg)|Gantry/Y|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="5"/>
-        <v>[![LDO Kit - Toolboard Mount v1](./images/printed_parts/Gantry/Y/LDO%20Kit%20-%20Toolboard%20Mount%20v1.jpg)]</v>
+        <v>![LDO Kit - Toolboard Mount v1](./images/printed_parts/Gantry/Y/LDO%20Kit%20-%20Toolboard%20Mount%20v1.jpg)</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="6"/>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
-        <v>|[LDO Kit - Toolboard Mount v1](../STLs/Gantry/Y/LDO%20Kit%20-%20Toolboard%20Mount%20v1.stl)|[![LDO Kit - Toolboard Mount v1](./images/printed_parts/Gantry/Y/LDO%20Kit%20-%20Toolboard%20Mount%20v1.jpg)]|Gantry/Y|Main|No|PLA or Better|</v>
+        <v>|[LDO Kit - Toolboard Mount v1](../STLs/Gantry/Y/LDO%20Kit%20-%20Toolboard%20Mount%20v1.stl)|![LDO Kit - Toolboard Mount v1](./images/printed_parts/Gantry/Y/LDO%20Kit%20-%20Toolboard%20Mount%20v1.jpg)|Gantry/Y|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v>[![BBProV25fl_LinearRailReplacement-MMU Painted Text](./images/printed_parts/Gantry/Y/MMU%20&amp;%20AMS/BBProV25fl_LinearRailReplacement-MMU%20Painted%20Text.3mf)]</v>
+        <v>![BBProV25fl_LinearRailReplacement-MMU Painted Text](./images/printed_parts/Gantry/Y/MMU%20&amp;%20AMS/BBProV25fl_LinearRailReplacement-MMU%20Painted%20Text.3mf)</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="6"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
-        <v>|[BBProV25fl_LinearRailReplacement-MMU Painted Text](../STLs/Gantry/Y/MMU%20&amp;%20AMS/BBProV25fl_LinearRailReplacement-MMU%20Painted%20Text.3mf)|[![BBProV25fl_LinearRailReplacement-MMU Painted Text](./images/printed_parts/Gantry/Y/MMU%20&amp;%20AMS/BBProV25fl_LinearRailReplacement-MMU%20Painted%20Text.3mf)]|Gantry/Y/MMU &amp; AMS|Main|No|PLA or Better|</v>
+        <v>|[BBProV25fl_LinearRailReplacement-MMU Painted Text](../STLs/Gantry/Y/MMU%20&amp;%20AMS/BBProV25fl_LinearRailReplacement-MMU%20Painted%20Text.3mf)|![BBProV25fl_LinearRailReplacement-MMU Painted Text](./images/printed_parts/Gantry/Y/MMU%20&amp;%20AMS/BBProV25fl_LinearRailReplacement-MMU%20Painted%20Text.3mf)|Gantry/Y/MMU &amp; AMS|Main|No|PLA or Better|</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_RockMonsterNo1YTentionerBody](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerBody.jpg)]</v>
+        <v>![[a]_BBProV25fl_RockMonsterNo1YTentionerBody](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerBody.jpg)</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="6"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_RockMonsterNo1YTentionerBody](../STLs/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerBody.stl)|[![[a]_BBProV25fl_RockMonsterNo1YTentionerBody](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerBody.jpg)]|Gantry/Y|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_RockMonsterNo1YTentionerBody](../STLs/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerBody.stl)|![[a]_BBProV25fl_RockMonsterNo1YTentionerBody](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerBody.jpg)|Gantry/Y|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder.jpg)]</v>
+        <v>![[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder.jpg)</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="6"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder](../STLs/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder.stl)|[![[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder.jpg)]|Gantry/Y|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder](../STLs/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder.stl)|![[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder](./images/printed_parts/Gantry/Y/[a]_BBProV25fl_RockMonsterNo1YTentionerIdlerHolder.jpg)|Gantry/Y|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_PrintBelt-Frame-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-A.jpg)]</v>
+        <v>![[a]_BBProV25fl_PrintBelt-Frame-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-A.jpg)</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="6"/>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_PrintBelt-Frame-A](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-A.stl)|[![[a]_BBProV25fl_PrintBelt-Frame-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-A.jpg)]|PrintBelt|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_PrintBelt-Frame-A](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-A.stl)|![[a]_BBProV25fl_PrintBelt-Frame-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-A.jpg)|PrintBelt|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_PrintBelt-Frame-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-B.jpg)]</v>
+        <v>![[a]_BBProV25fl_PrintBelt-Frame-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-B.jpg)</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="6"/>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_PrintBelt-Frame-B](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-B.stl)|[![[a]_BBProV25fl_PrintBelt-Frame-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-B.jpg)]|PrintBelt|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_PrintBelt-Frame-B](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-B.stl)|![[a]_BBProV25fl_PrintBelt-Frame-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Frame-B.jpg)|PrintBelt|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_PrintBelt-Nut(2x)](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Nut(2x).jpg)]</v>
+        <v>![[a]_BBProV25fl_PrintBelt-Nut(2x)](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Nut(2x).jpg)</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="6"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_PrintBelt-Nut(2x)](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Nut(2x).stl)|[![[a]_BBProV25fl_PrintBelt-Nut(2x)](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Nut(2x).jpg)]|PrintBelt|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_PrintBelt-Nut(2x)](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Nut(2x).stl)|![[a]_BBProV25fl_PrintBelt-Nut(2x)](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Nut(2x).jpg)|PrintBelt|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_PrintBelt-Pusher-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-A.jpg)]</v>
+        <v>![[a]_BBProV25fl_PrintBelt-Pusher-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-A.jpg)</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="6"/>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_PrintBelt-Pusher-A](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-A.stl)|[![[a]_BBProV25fl_PrintBelt-Pusher-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-A.jpg)]|PrintBelt|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_PrintBelt-Pusher-A](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-A.stl)|![[a]_BBProV25fl_PrintBelt-Pusher-A](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-A.jpg)|PrintBelt|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1782,7 +1782,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_PrintBelt-Pusher-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-B.jpg)]</v>
+        <v>![[a]_BBProV25fl_PrintBelt-Pusher-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-B.jpg)</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="6"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_PrintBelt-Pusher-B](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-B.stl)|[![[a]_BBProV25fl_PrintBelt-Pusher-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-B.jpg)]|PrintBelt|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_PrintBelt-Pusher-B](../STLs/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-B.stl)|![[a]_BBProV25fl_PrintBelt-Pusher-B](./images/printed_parts/PrintBelt/[a]_BBProV25fl_PrintBelt-Pusher-B.jpg)|PrintBelt|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="5"/>
-        <v>[![[any]_BBPro_XRailSpacerV2[x2]](./images/printed_parts/Tools/[any]_BBPro_XRailSpacerV2[x2].jpg)]</v>
+        <v>![[any]_BBPro_XRailSpacerV2[x2]](./images/printed_parts/Tools/[any]_BBPro_XRailSpacerV2[x2].jpg)</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="6"/>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="K32" t="str">
         <f t="shared" si="1"/>
-        <v>|[[any]_BBPro_XRailSpacerV2[x2]](../STLs/Tools/[any]_BBPro_XRailSpacerV2[x2].stl)|[![[any]_BBPro_XRailSpacerV2[x2]](./images/printed_parts/Tools/[any]_BBPro_XRailSpacerV2[x2].jpg)]|Tools|Accent|No|PLA or Better|</v>
+        <v>|[[any]_BBPro_XRailSpacerV2[x2]](../STLs/Tools/[any]_BBPro_XRailSpacerV2[x2].stl)|![[any]_BBPro_XRailSpacerV2[x2]](./images/printed_parts/Tools/[any]_BBPro_XRailSpacerV2[x2].jpg)|Tools|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a,s]_BBProV25fl_Roller[x2]](./images/printed_parts/ZBeltDrive/[a,s]_BBProV25fl_Roller[x2].jpg)]</v>
+        <v>![[a,s]_BBProV25fl_Roller[x2]](./images/printed_parts/ZBeltDrive/[a,s]_BBProV25fl_Roller[x2].jpg)</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="6"/>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="K33" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a,s]_BBProV25fl_Roller[x2]](../STLs/ZBeltDrive/[a,s]_BBProV25fl_Roller[x2].stl)|[![[a,s]_BBProV25fl_Roller[x2]](./images/printed_parts/ZBeltDrive/[a,s]_BBProV25fl_Roller[x2].jpg)]|ZBeltDrive|Accent|Yes|PLA or Better|</v>
+        <v>|[[a,s]_BBProV25fl_Roller[x2]](../STLs/ZBeltDrive/[a,s]_BBProV25fl_Roller[x2].stl)|![[a,s]_BBProV25fl_Roller[x2]](./images/printed_parts/ZBeltDrive/[a,s]_BBProV25fl_Roller[x2].jpg)|ZBeltDrive|Accent|Yes|PLA or Better|</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_Nema17_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Nema17_ZGear.jpg)]</v>
+        <v>![[a]_BBProV25fl_Nema17_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Nema17_ZGear.jpg)</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="6"/>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="K34" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_Nema17_ZGear](../STLs/ZBeltDrive/[a]_BBProV25fl_Nema17_ZGear.stl)|[![[a]_BBProV25fl_Nema17_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Nema17_ZGear.jpg)]|ZBeltDrive|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_Nema17_ZGear](../STLs/ZBeltDrive/[a]_BBProV25fl_Nema17_ZGear.stl)|![[a]_BBProV25fl_Nema17_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Nema17_ZGear.jpg)|ZBeltDrive|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="5"/>
-        <v>[![[a]_BBProV25fl_Roller_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Roller_ZGear.jpg)]</v>
+        <v>![[a]_BBProV25fl_Roller_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Roller_ZGear.jpg)</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="6"/>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="K35" t="str">
         <f t="shared" si="1"/>
-        <v>|[[a]_BBProV25fl_Roller_ZGear](../STLs/ZBeltDrive/[a]_BBProV25fl_Roller_ZGear.stl)|[![[a]_BBProV25fl_Roller_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Roller_ZGear.jpg)]|ZBeltDrive|Accent|No|PLA or Better|</v>
+        <v>|[[a]_BBProV25fl_Roller_ZGear](../STLs/ZBeltDrive/[a]_BBProV25fl_Roller_ZGear.stl)|![[a]_BBProV25fl_Roller_ZGear](./images/printed_parts/ZBeltDrive/[a]_BBProV25fl_Roller_ZGear.jpg)|ZBeltDrive|Accent|No|PLA or Better|</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="5"/>
-        <v>[![[HT]_BBProV25fl_UnderbedOrBed](./images/printed_parts/ZBeltDrive/[HT]_BBProV25fl_UnderbedOrBed.jpg)]</v>
+        <v>![[HT]_BBProV25fl_UnderbedOrBed](./images/printed_parts/ZBeltDrive/[HT]_BBProV25fl_UnderbedOrBed.jpg)</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="6"/>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="K36" t="str">
         <f t="shared" si="1"/>
-        <v>|[[HT]_BBProV25fl_UnderbedOrBed](../STLs/ZBeltDrive/[HT]_BBProV25fl_UnderbedOrBed.stl)|[![[HT]_BBProV25fl_UnderbedOrBed](./images/printed_parts/ZBeltDrive/[HT]_BBProV25fl_UnderbedOrBed.jpg)]|ZBeltDrive|Main|No|PLA or Better|</v>
+        <v>|[[HT]_BBProV25fl_UnderbedOrBed](../STLs/ZBeltDrive/[HT]_BBProV25fl_UnderbedOrBed.stl)|![[HT]_BBProV25fl_UnderbedOrBed](./images/printed_parts/ZBeltDrive/[HT]_BBProV25fl_UnderbedOrBed.jpg)|ZBeltDrive|Main|No|PLA or Better|</v>
       </c>
     </row>
   </sheetData>

</xml_diff>